<commit_message>
updated helpers and components
</commit_message>
<xml_diff>
--- a/public/textBook.xlsx
+++ b/public/textBook.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\accounting\accounting_fe\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5791B66B-A923-436D-84B3-C508A3EBB55E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FFE2BCE-1F29-4F5C-B7BF-3069D98F23BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Книга облику" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -222,25 +222,25 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -526,7 +526,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -542,15 +542,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="12"/>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
     </row>
     <row r="2" spans="1:9" ht="75.599999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
@@ -564,37 +564,37 @@
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="11"/>
-      <c r="F2" s="9"/>
+      <c r="F2" s="12"/>
       <c r="G2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="9"/>
+      <c r="H2" s="12"/>
       <c r="I2" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="114.6" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7" t="s">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="6"/>
+      <c r="I3" s="9"/>
     </row>
     <row r="4" spans="1:9" ht="22.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
@@ -625,7 +625,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="67.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="40.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>1</v>
       </c>

</xml_diff>